<commit_message>
MBasicInt and copilot instructions
</commit_message>
<xml_diff>
--- a/data/EX_MBasic.xlsx
+++ b/data/EX_MBasic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\lpEnergyModels\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E219037F-8128-4037-A9C5-BF8897376B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD618EF-E913-4476-A6E4-B74BDB4DADE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>